<commit_message>
Demo values in excel files
</commit_message>
<xml_diff>
--- a/SDS2.0Metadata/code_parameters.xlsx
+++ b/SDS2.0Metadata/code_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nalo1\2022-project-2\SDS2.0Metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FC9EC2-CCCD-4D83-860D-32B0D0402581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A44157-DC19-4A82-B980-1119661B7D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Type</t>
   </si>
@@ -109,7 +109,10 @@
     <t>Frequency</t>
   </si>
   <si>
-    <t>Heat</t>
+    <t>Sound</t>
+  </si>
+  <si>
+    <t>Temperature</t>
   </si>
 </sst>
 </file>
@@ -597,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -616,7 +619,7 @@
     <col min="9" max="9" width="16.81640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -653,8 +656,9 @@
       <c r="L1" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="M1" s="6"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -693,13 +697,27 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Connection and commenting changes
</commit_message>
<xml_diff>
--- a/SDS2.0Metadata/code_parameters.xlsx
+++ b/SDS2.0Metadata/code_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nalo1\2022-project-2\SDS2.0Metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A44157-DC19-4A82-B980-1119661B7D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400400DE-263A-4976-AB9E-8EA16A7B9D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Type</t>
   </si>
@@ -113,6 +113,15 @@
   </si>
   <si>
     <t>Temperature</t>
+  </si>
+  <si>
+    <t>hz</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>dB</t>
   </si>
 </sst>
 </file>
@@ -603,7 +612,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -704,6 +713,12 @@
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="1">
+        <v>50</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -712,6 +727,12 @@
       <c r="B4" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="1">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -719,6 +740,12 @@
       </c>
       <c r="B5" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="1">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>